<commit_message>
Add data from tests Excel
</commit_message>
<xml_diff>
--- a/VerificationData/TestingDescription.xlsx
+++ b/VerificationData/TestingDescription.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fkakg\Documents\Visual Studio 2017\Projects\FlowCalibration\VerificationData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fredrik Schyum\Documents\Skola\SSY226\code\FlowCalibrationUserInterface\VerificationData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7530" xr2:uid="{80BB5024-C267-4B83-B601-05778BD4DD24}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Tests to be run" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Blad1" sheetId="1" r:id="rId3"/>
+    <sheet name="Blad2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="Blad1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Blad1!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Blad1!$A$1:$O$1</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="135">
   <si>
     <t>ID</t>
   </si>
@@ -253,9 +254,6 @@
     <t>Each case is repeated 3 times</t>
   </si>
   <si>
-    <t>Sample rate for all cases is 0.035s</t>
-  </si>
-  <si>
     <t>Sine wave, 1 period, frequency 1, amplitude 2</t>
   </si>
   <si>
@@ -274,9 +272,6 @@
     <t>Distance between the sled and the syringe is measured with a caliper</t>
   </si>
   <si>
-    <t>Sample rate is 0.035s</t>
-  </si>
-  <si>
     <t>Square wave, 0.5 periods, frequency 6, amplitude 200, padded with zeros</t>
   </si>
   <si>
@@ -386,13 +381,70 @@
   </si>
   <si>
     <t>Each case is repeated 1 times</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>Amp 200 F 14 10 rep</t>
+  </si>
+  <si>
+    <t>Innan</t>
+  </si>
+  <si>
+    <t>Efter</t>
+  </si>
+  <si>
+    <t>Data [ml]</t>
+  </si>
+  <si>
+    <t>% error</t>
+  </si>
+  <si>
+    <t>dV [ml]</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Max Vol</t>
+  </si>
+  <si>
+    <t>Av Ants</t>
+  </si>
+  <si>
+    <t>65,8/65,7/67,82 kvar med init botten</t>
+  </si>
+  <si>
+    <t>74/71/70 kvar med init botten</t>
+  </si>
+  <si>
+    <t>13,2/13,5/13,5 kvar med init nästan i botten</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>Max flow nästan 200</t>
+  </si>
+  <si>
+    <t>Vol ca 22-26</t>
+  </si>
+  <si>
+    <t>Vid låga flöden och snabb sampling påverkar upplösningen på motorn och gör flödessignalen brusig</t>
+  </si>
+  <si>
+    <t>Sample rate is 0.040s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,6 +454,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -503,10 +562,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -546,9 +606,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Procent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -564,7 +626,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -859,64 +921,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D4CBC7-13D4-4373-A0F4-19C179C68A27}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="7" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>114</v>
-      </c>
       <c r="L1" s="11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="13" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="13" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>71</v>
@@ -928,29 +990,29 @@
         <v>73</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -959,12 +1021,12 @@
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
     </row>
-    <row r="4" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -973,12 +1035,12 @@
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
     </row>
-    <row r="5" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -987,7 +1049,7 @@
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
     </row>
-    <row r="6" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
@@ -995,41 +1057,41 @@
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
     </row>
-    <row r="7" spans="1:12" s="13" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="13" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>79</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>80</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>73</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J7" s="14"/>
       <c r="K7" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L7" s="14"/>
     </row>
-    <row r="8" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
@@ -1038,12 +1100,12 @@
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
     </row>
-    <row r="9" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
@@ -1052,12 +1114,12 @@
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
     </row>
-    <row r="10" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
@@ -1066,7 +1128,7 @@
       <c r="K10" s="16"/>
       <c r="L10" s="16"/>
     </row>
-    <row r="11" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
@@ -1074,41 +1136,41 @@
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
     </row>
-    <row r="12" spans="1:12" s="13" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="13" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>87</v>
-      </c>
       <c r="D12" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
       <c r="K12" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L12" s="14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
@@ -1117,12 +1179,12 @@
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
     </row>
-    <row r="14" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
@@ -1131,12 +1193,12 @@
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
     </row>
-    <row r="15" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
@@ -1145,7 +1207,7 @@
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
     </row>
-    <row r="16" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
@@ -1153,77 +1215,84 @@
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
     </row>
-    <row r="17" spans="1:12" s="13" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="13" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>96</v>
-      </c>
       <c r="D17" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
     </row>
-    <row r="18" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B20" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+    <row r="22" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="B22" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="23" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1231,23 +1300,396 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395EBB35-3F2D-47E0-83BB-88CF0B379EC8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M1">
+        <f>1.7^2*PI()</f>
+        <v>9.0792027688745005</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>97.25</v>
+      </c>
+      <c r="D2">
+        <v>26.4</v>
+      </c>
+      <c r="E2">
+        <v>65.894999999999996</v>
+      </c>
+      <c r="F2">
+        <f>(C2-D2)/10*$M$1</f>
+        <v>64.32615161747583</v>
+      </c>
+      <c r="G2" s="17">
+        <f>E2/F2-1</f>
+        <v>2.4388966898774456E-2</v>
+      </c>
+      <c r="H2" s="11">
+        <f>E2-F2</f>
+        <v>1.5688483825241661</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>96.5</v>
+      </c>
+      <c r="D3">
+        <v>23.1</v>
+      </c>
+      <c r="E3">
+        <v>67.165000000000006</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F10" si="0">(C3-D3)/10*$M$1</f>
+        <v>66.641348323538836</v>
+      </c>
+      <c r="G3" s="17">
+        <f t="shared" ref="G3:G10" si="1">E3/F3-1</f>
+        <v>7.8577593286210945E-3</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H10" si="2">E3-F3</f>
+        <v>0.52365167646117072</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>98.4</v>
+      </c>
+      <c r="D4">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>66.213999999999999</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>65.733428046651383</v>
+      </c>
+      <c r="G4" s="17">
+        <f t="shared" si="1"/>
+        <v>7.3109218190712255E-3</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>0.48057195334861547</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>73.3</v>
+      </c>
+      <c r="D5">
+        <v>73.05</v>
+      </c>
+      <c r="E5">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.22698006922186253</v>
+      </c>
+      <c r="G5" s="17">
+        <f t="shared" si="1"/>
+        <v>-0.22019584976427753</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>-4.9980069221862544E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>73.05</v>
+      </c>
+      <c r="D6">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="E6">
+        <v>0.156</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.13618804153310976</v>
+      </c>
+      <c r="G6" s="17">
+        <f t="shared" si="1"/>
+        <v>0.14547502294519443</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>1.9811958466890239E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="D7">
+        <v>72.849999999999994</v>
+      </c>
+      <c r="E7">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>4.5396013844382826E-2</v>
+      </c>
+      <c r="G7" s="17">
+        <f t="shared" si="1"/>
+        <v>2.5906236296156466</v>
+      </c>
+      <c r="H7" s="11">
+        <f t="shared" si="2"/>
+        <v>0.11760398615561718</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="D8">
+        <v>50.6</v>
+      </c>
+      <c r="E8">
+        <v>20.747</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>20.24662217459014</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="1"/>
+        <v>2.4714138540987918E-2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>0.50037782540985987</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>67.25</v>
+      </c>
+      <c r="D9">
+        <v>44.25</v>
+      </c>
+      <c r="E9">
+        <v>21.024000000000001</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>20.882166368411351</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="1"/>
+        <v>6.7920937457524033E-3</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>0.14183363158864992</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>90.75</v>
+      </c>
+      <c r="D10">
+        <v>68.2</v>
+      </c>
+      <c r="E10">
+        <v>20.74</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>20.473602243811996</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" si="1"/>
+        <v>1.3011767690686682E-2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>0.26639775618800243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" t="s">
+        <v>128</v>
+      </c>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" t="s">
+        <v>129</v>
+      </c>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B19" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B20" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20" s="17"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="41.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.453125" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>46</v>
       </c>
@@ -1264,32 +1706,32 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1297,7 +1739,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -1305,7 +1747,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>55</v>
       </c>
@@ -1313,7 +1755,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1321,7 +1763,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -1329,7 +1771,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -1337,12 +1779,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1350,7 +1792,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -1358,7 +1800,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -1372,35 +1814,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB38A0D6-F902-4601-95BD-04132A3D3D3C}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="26.26953125" customWidth="1"/>
+    <col min="4" max="4" width="24.453125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" style="3" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.81640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" customWidth="1"/>
+    <col min="13" max="13" width="9.7265625" customWidth="1"/>
+    <col min="14" max="14" width="10.1796875" customWidth="1"/>
+    <col min="15" max="15" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="7" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="7" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1447,37 +1889,37 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>18</v>
       </c>
@@ -1505,7 +1947,7 @@
       <c r="I8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>24</v>
       </c>
@@ -1533,7 +1975,7 @@
       <c r="I9" s="9"/>
       <c r="K9" s="9"/>
     </row>
-    <row r="10" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>25</v>
       </c>
@@ -1561,7 +2003,7 @@
       <c r="I10" s="9"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>26</v>
       </c>
@@ -1589,7 +2031,7 @@
       <c r="I11" s="9"/>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>18</v>
       </c>
@@ -1617,7 +2059,7 @@
       <c r="I12" s="9"/>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>24</v>
       </c>
@@ -1645,7 +2087,7 @@
       <c r="I13" s="9"/>
       <c r="K13" s="9"/>
     </row>
-    <row r="14" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>25</v>
       </c>
@@ -1673,7 +2115,7 @@
       <c r="I14" s="9"/>
       <c r="K14" s="9"/>
     </row>
-    <row r="15" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>26</v>
       </c>
@@ -1701,12 +2143,12 @@
       <c r="I15" s="9"/>
       <c r="K15" s="9"/>
     </row>
-    <row r="16" spans="1:15" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Add matlab error and std analysis
</commit_message>
<xml_diff>
--- a/VerificationData/TestingDescription.xlsx
+++ b/VerificationData/TestingDescription.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tests to be run" sheetId="3" r:id="rId1"/>
-    <sheet name="Blad2" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
-    <sheet name="Blad1" sheetId="1" r:id="rId4"/>
+    <sheet name="Blad3" sheetId="5" r:id="rId2"/>
+    <sheet name="Blad2" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
+    <sheet name="Blad1" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Blad1!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Blad1!$A$1:$O$1</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="151">
   <si>
     <t>ID</t>
   </si>
@@ -435,6 +436,54 @@
   </si>
   <si>
     <t>Sample rate is 0.040s</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>Front</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Front - something</t>
+  </si>
+  <si>
+    <t>Three way - something</t>
+  </si>
+  <si>
+    <t>Medel</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>Medel/Vol</t>
+  </si>
+  <si>
+    <t>Median/Vol</t>
+  </si>
+  <si>
+    <t>STD/Vol</t>
+  </si>
+  <si>
+    <t>Ointressanta siffror?</t>
+  </si>
+  <si>
+    <t>Two way - Almost nothing. Similar error affecting both directions</t>
   </si>
 </sst>
 </file>
@@ -444,7 +493,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,6 +512,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -494,7 +550,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -561,12 +617,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -607,6 +672,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -924,9 +1002,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1301,10 +1379,482 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="8.7265625" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="O1" t="s">
+        <v>124</v>
+      </c>
+      <c r="P1">
+        <f>1.7^2*PI()</f>
+        <v>9.0792027688745005</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>97.25</v>
+      </c>
+      <c r="D2">
+        <v>26.4</v>
+      </c>
+      <c r="E2">
+        <v>65.894999999999996</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F10" si="0">(C2-D2)/10*$P$1</f>
+        <v>64.32615161747583</v>
+      </c>
+      <c r="G2" s="17">
+        <f>E2/F2-1</f>
+        <v>2.4388966898774456E-2</v>
+      </c>
+      <c r="H2" s="11">
+        <f>E2-F2</f>
+        <v>1.5688483825241661</v>
+      </c>
+      <c r="I2" s="19">
+        <f>AVERAGE(H2:H4)</f>
+        <v>0.85769067077798411</v>
+      </c>
+      <c r="J2" s="28">
+        <f>MEDIAN(H2:H4)</f>
+        <v>0.52365167646117072</v>
+      </c>
+      <c r="K2">
+        <f>_xlfn.STDEV.P(H2:H4)</f>
+        <v>0.50317189499408854</v>
+      </c>
+      <c r="L2" s="17">
+        <f>AVERAGE(H2/F2,H3/F3,H4/F4)</f>
+        <v>1.3185882682155592E-2</v>
+      </c>
+      <c r="M2" s="17">
+        <f>MEDIAN(H2/F2,H3/F3,H4/F4)</f>
+        <v>7.8577593286210303E-3</v>
+      </c>
+      <c r="N2" s="17">
+        <f>_xlfn.STDEV.P(H2/F2,H3/F3,H4/F4)</f>
+        <v>7.9249218624519759E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>96.5</v>
+      </c>
+      <c r="D3">
+        <v>23.1</v>
+      </c>
+      <c r="E3">
+        <v>67.165000000000006</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>66.641348323538836</v>
+      </c>
+      <c r="G3" s="17">
+        <f t="shared" ref="G3:G10" si="1">E3/F3-1</f>
+        <v>7.8577593286210945E-3</v>
+      </c>
+      <c r="H3">
+        <f>E3-F3</f>
+        <v>0.52365167646117072</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>98.4</v>
+      </c>
+      <c r="D4">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>66.213999999999999</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>65.733428046651383</v>
+      </c>
+      <c r="G4" s="17">
+        <f t="shared" si="1"/>
+        <v>7.3109218190712255E-3</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H10" si="2">E4-F4</f>
+        <v>0.48057195334861547</v>
+      </c>
+      <c r="I4" s="19"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="22">
+        <v>2</v>
+      </c>
+      <c r="B5" s="22">
+        <v>1</v>
+      </c>
+      <c r="C5" s="22">
+        <v>73.3</v>
+      </c>
+      <c r="D5" s="22">
+        <v>73.05</v>
+      </c>
+      <c r="E5" s="22">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="F5" s="22">
+        <f t="shared" si="0"/>
+        <v>0.22698006922186253</v>
+      </c>
+      <c r="G5" s="23">
+        <f t="shared" si="1"/>
+        <v>-0.22019584976427753</v>
+      </c>
+      <c r="H5" s="22">
+        <f t="shared" si="2"/>
+        <v>-4.9980069221862544E-2</v>
+      </c>
+      <c r="I5" s="26">
+        <f t="shared" ref="I5:I8" si="3">AVERAGE(H5:H7)</f>
+        <v>2.9145291800214957E-2</v>
+      </c>
+      <c r="J5" s="28">
+        <f t="shared" ref="J5:J8" si="4">MEDIAN(H5:H7)</f>
+        <v>1.9811958466890239E-2</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K8" si="5">_xlfn.STDEV.P(H5:H7)</f>
+        <v>6.8733481591452261E-2</v>
+      </c>
+      <c r="L5" s="30">
+        <f>AVERAGE(H5/F5,H6/F6,H7/F7)</f>
+        <v>0.83863426759885451</v>
+      </c>
+      <c r="M5" s="30">
+        <f>MEDIAN(H5/F5,H6/F6,H7/F7)</f>
+        <v>0.14547502294519446</v>
+      </c>
+      <c r="N5" s="30">
+        <f>_xlfn.STDEV.P(H5/F5,H6/F6,H7/F7)</f>
+        <v>1.2478057648667469</v>
+      </c>
+      <c r="O5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22">
+        <v>2</v>
+      </c>
+      <c r="C6" s="22">
+        <v>73.05</v>
+      </c>
+      <c r="D6" s="22">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="E6" s="22">
+        <v>0.156</v>
+      </c>
+      <c r="F6" s="22">
+        <f t="shared" si="0"/>
+        <v>0.13618804153310976</v>
+      </c>
+      <c r="G6" s="23">
+        <f t="shared" si="1"/>
+        <v>0.14547502294519443</v>
+      </c>
+      <c r="H6" s="22">
+        <f t="shared" si="2"/>
+        <v>1.9811958466890239E-2</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22">
+        <v>3</v>
+      </c>
+      <c r="C7" s="22">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="D7" s="22">
+        <v>72.849999999999994</v>
+      </c>
+      <c r="E7" s="22">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="F7" s="22">
+        <f t="shared" si="0"/>
+        <v>4.5396013844382826E-2</v>
+      </c>
+      <c r="G7" s="23">
+        <f t="shared" si="1"/>
+        <v>2.5906236296156466</v>
+      </c>
+      <c r="H7" s="24">
+        <f t="shared" si="2"/>
+        <v>0.11760398615561718</v>
+      </c>
+      <c r="I7" s="26"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="D8">
+        <v>50.6</v>
+      </c>
+      <c r="E8">
+        <v>20.747</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>20.24662217459014</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="1"/>
+        <v>2.4714138540987918E-2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>0.50037782540985987</v>
+      </c>
+      <c r="I8" s="19">
+        <f t="shared" si="3"/>
+        <v>0.30286973772883741</v>
+      </c>
+      <c r="J8" s="28">
+        <f t="shared" si="4"/>
+        <v>0.26639775618800243</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="5"/>
+        <v>0.14862960406967293</v>
+      </c>
+      <c r="L8" s="20">
+        <f>AVERAGE(H8/F8,H9/F9,H10/F10)</f>
+        <v>1.4839333325809036E-2</v>
+      </c>
+      <c r="M8" s="20">
+        <f>MEDIAN(H8/F8,H9/F9,H10/F10)</f>
+        <v>1.301176769068664E-2</v>
+      </c>
+      <c r="N8" s="20">
+        <f>_xlfn.STDEV.P(H8/F8,H9/F9,H10/F10)</f>
+        <v>7.4298909603312049E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>67.25</v>
+      </c>
+      <c r="D9">
+        <v>44.25</v>
+      </c>
+      <c r="E9">
+        <v>21.024000000000001</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>20.882166368411351</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="1"/>
+        <v>6.7920937457524033E-3</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>0.14183363158864992</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="L9" s="18">
+        <f>AVERAGE(L8,L2)</f>
+        <v>1.4012608003982314E-2</v>
+      </c>
+      <c r="M9" s="18">
+        <f t="shared" ref="M9:N9" si="6">AVERAGE(M8,M2)</f>
+        <v>1.0434763509653836E-2</v>
+      </c>
+      <c r="N9" s="18">
+        <f t="shared" si="6"/>
+        <v>7.6774064113915904E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>90.75</v>
+      </c>
+      <c r="D10">
+        <v>68.2</v>
+      </c>
+      <c r="E10">
+        <v>20.74</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>20.473602243811996</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" si="1"/>
+        <v>1.3011767690686682E-2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>0.26639775618800243</v>
+      </c>
+      <c r="I10" s="19"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="29"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="29"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="29"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1367,6 +1917,14 @@
         <f>E2-F2</f>
         <v>1.5688483825241661</v>
       </c>
+      <c r="I2" s="19">
+        <f>AVERAGE(H2:H4)</f>
+        <v>0.85769067077798411</v>
+      </c>
+      <c r="J2" s="18">
+        <f>AVERAGE(G2:G4)</f>
+        <v>1.3185882682155592E-2</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B3">
@@ -1393,6 +1951,8 @@
         <f t="shared" ref="H3:H10" si="2">E3-F3</f>
         <v>0.52365167646117072</v>
       </c>
+      <c r="I3" s="19"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B4">
@@ -1419,6 +1979,8 @@
         <f t="shared" si="2"/>
         <v>0.48057195334861547</v>
       </c>
+      <c r="I4" s="19"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -1448,6 +2010,20 @@
         <f t="shared" si="2"/>
         <v>-4.9980069221862544E-2</v>
       </c>
+      <c r="I5" s="19">
+        <f t="shared" ref="I5:I8" si="3">AVERAGE(H5:H7)</f>
+        <v>2.9145291800214957E-2</v>
+      </c>
+      <c r="J5" s="18">
+        <f t="shared" ref="J5:J8" si="4">AVERAGE(G5:G7)</f>
+        <v>0.83863426759885451</v>
+      </c>
+      <c r="K5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B6">
@@ -1474,6 +2050,14 @@
         <f t="shared" si="2"/>
         <v>1.9811958466890239E-2</v>
       </c>
+      <c r="I6" s="19"/>
+      <c r="J6" s="18"/>
+      <c r="K6" t="s">
+        <v>137</v>
+      </c>
+      <c r="L6" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B7">
@@ -1500,6 +2084,14 @@
         <f t="shared" si="2"/>
         <v>0.11760398615561718</v>
       </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="18"/>
+      <c r="K7" t="s">
+        <v>138</v>
+      </c>
+      <c r="L7" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -1529,6 +2121,14 @@
         <f t="shared" si="2"/>
         <v>0.50037782540985987</v>
       </c>
+      <c r="I8" s="19">
+        <f t="shared" si="3"/>
+        <v>0.30286973772883741</v>
+      </c>
+      <c r="J8" s="18">
+        <f t="shared" si="4"/>
+        <v>1.4839333325809001E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B9">
@@ -1555,6 +2155,7 @@
         <f t="shared" si="2"/>
         <v>0.14183363158864992</v>
       </c>
+      <c r="I9" s="19"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B10">
@@ -1581,9 +2182,13 @@
         <f t="shared" si="2"/>
         <v>0.26639775618800243</v>
       </c>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="G11" s="17"/>
+      <c r="G11" s="17">
+        <f>MEDIAN(G8:G10,G2:G4)</f>
+        <v>1.0434763509653888E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -1640,7 +2245,13 @@
       <c r="B17" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="G17" s="17"/>
+      <c r="F17">
+        <f>14/2/PI()</f>
+        <v>2.228169203286535</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -1674,7 +2285,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
@@ -1814,7 +2425,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O20"/>
   <sheetViews>

</xml_diff>